<commit_message>
Updated after review with em-micro team
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/emus-CV32E40P_instruction_exceptions.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/emus-CV32E40P_instruction_exceptions.xlsx
@@ -8,15 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF35AA41-D24A-468C-A61C-906465054A0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B07E09-DF6A-4065-8690-DF1F620C86FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vplan" sheetId="1" r:id="rId1"/>
     <sheet name="Permutations" sheetId="2" r:id="rId2"/>
-    <sheet name="EBREAK" sheetId="3" r:id="rId3"/>
-    <sheet name="CSRs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,8 +40,6 @@
     <author>tc={DD7F894F-9234-45F3-8684-F5714E6F9F00}</author>
     <author>tc={89B78706-C4A4-4214-92F5-A0D38D74FF9E}</author>
     <author>tc={F5DE54AA-7939-4D93-9554-653FB95AB5D1}</author>
-    <author>tc={B5686705-6936-4530-B6D0-3F3CD5963FE2}</author>
-    <author>tc={6E6FDA3F-C3C0-43D6-ADD6-7422FC32A68B}</author>
     <author>tc={4D7114F4-5E6B-4775-AE24-3DDEAA3CDBB2}</author>
     <author>tc={E64922F1-6739-4F8C-9676-630AF88E031E}</author>
     <author>tc={09651DE0-A277-480B-A8D0-FD376075F849}</author>
@@ -55,7 +51,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Its not clear that this a feature of CV32E40P.  I've open issue #497 to find out.</t>
+    Its not clear that this a feature of CV32E40P.  I've open issue #497 to find out.
+Reply:
+    Need to add the concept of "non-existant addresses" in the testbench memory.</t>
       </text>
     </comment>
     <comment ref="B3" authorId="1" shapeId="0" xr:uid="{FD0C4767-67A6-4F9E-8956-3FCB07F9ED56}">
@@ -63,7 +61,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    How do we present illegal instructions to the core?  Will the Google ISG actually generate illegal instructions?   How are these handled by the toolchain?</t>
+    How do we present illegal instructions to the core?  Will the Google ISG actually generate illegal instructions?   How are these handled by the toolchain?
+Reply:
+    David has a script that deliberately generates mis-formed instructions.</t>
       </text>
     </comment>
     <comment ref="B4" authorId="2" shapeId="0" xr:uid="{9D2A13B5-1671-4066-99D0-5AAEE72AF6AF}">
@@ -79,7 +79,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Question: can your test-program throw an error if an unexpected exception occurs?   Throw an error if an expected exception does not occur?</t>
+    Question: can your test-program throw an error if an unexpected exception occurs?   Throw an error if an expected exception does not occur?
+Reply:
+    Not required - ISS will mis-match on mepc</t>
       </text>
     </comment>
     <comment ref="G6" authorId="4" shapeId="0" xr:uid="{2406D81D-9721-4D0D-B869-47006E696B60}">
@@ -87,7 +89,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Idealy we would have functional coverage on the Instruction fetch bus to cover these specific scenarios.</t>
+    Idealy we would have functional coverage on the Instruction fetch bus to cover these specific scenarios.
+Reply:
+    All agreed.</t>
       </text>
     </comment>
     <comment ref="B8" authorId="5" shapeId="0" xr:uid="{4AD939A8-000B-4C00-9781-6690334399AA}">
@@ -135,7 +139,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    I like this Feature, but its not clear how the test-program is implemented.</t>
+    I like this Feature, but its not clear how the test-program is implemented.
+Reply:
+    Two options: (1) encode the expected exception in the handler, or (2) compare against RM.</t>
       </text>
     </comment>
     <comment ref="C23" authorId="11" shapeId="0" xr:uid="{F5DE54AA-7939-4D93-9554-653FB95AB5D1}">
@@ -146,23 +152,7 @@
     Ordinarily this would be part of a CSR DV plan, but getting bits set in mcause is better done as part of the exceptions DV plan.</t>
       </text>
     </comment>
-    <comment ref="D23" authorId="12" shapeId="0" xr:uid="{B5686705-6936-4530-B6D0-3F3CD5963FE2}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    PoR value of mstatus is 0x1800.  PoR of mcause is 0x0.</t>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="13" shapeId="0" xr:uid="{6E6FDA3F-C3C0-43D6-ADD6-7422FC32A68B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This should be reset after some exception causes mcause to be non-zero.</t>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="14" shapeId="0" xr:uid="{4D7114F4-5E6B-4775-AE24-3DDEAA3CDBB2}">
+    <comment ref="B24" authorId="12" shapeId="0" xr:uid="{4D7114F4-5E6B-4775-AE24-3DDEAA3CDBB2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +160,7 @@
     Debug DV plan</t>
       </text>
     </comment>
-    <comment ref="B25" authorId="15" shapeId="0" xr:uid="{E64922F1-6739-4F8C-9676-630AF88E031E}">
+    <comment ref="B25" authorId="13" shapeId="0" xr:uid="{E64922F1-6739-4F8C-9676-630AF88E031E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -178,7 +168,7 @@
     Debug DV plan</t>
       </text>
     </comment>
-    <comment ref="B26" authorId="16" shapeId="0" xr:uid="{09651DE0-A277-480B-A8D0-FD376075F849}">
+    <comment ref="B26" authorId="14" shapeId="0" xr:uid="{09651DE0-A277-480B-A8D0-FD376075F849}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -186,7 +176,7 @@
     Maybe already covered in Debug plan (need to check).</t>
       </text>
     </comment>
-    <comment ref="B27" authorId="17" shapeId="0" xr:uid="{71674E71-FADC-4E2B-8E72-9FEE78F17001}">
+    <comment ref="B27" authorId="15" shapeId="0" xr:uid="{71674E71-FADC-4E2B-8E72-9FEE78F17001}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -199,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="171">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -347,9 +337,6 @@
     <t>Check that mtval ignores writes and reads 0 and does not generate exceptions</t>
   </si>
   <si>
-    <t>Show that mcause is the correct value upon reset (0x00001800)</t>
-  </si>
-  <si>
     <t>Show that mcause has correct values when exceptions occur</t>
   </si>
   <si>
@@ -399,9 +386,6 @@
   </si>
   <si>
     <t>Ecall, ebreak, and c.ebreak all generate the appropriate exceptions</t>
-  </si>
-  <si>
-    <t>Reset sets mcause to 0x00001800</t>
   </si>
   <si>
     <t>Demonstrate that instruction values that don’t have an associated functionality generate an illegal instruction exception when run</t>
@@ -627,66 +611,6 @@
     <t>Internal signal riscv_core/debug_mode=1</t>
   </si>
   <si>
-    <t>FW</t>
-  </si>
-  <si>
-    <t>Main code:</t>
-  </si>
-  <si>
-    <t>Do some code</t>
-  </si>
-  <si>
-    <t>issue wfi to sleep/wait</t>
-  </si>
-  <si>
-    <t>do some code</t>
-  </si>
-  <si>
-    <t>First Debug handler:</t>
-  </si>
-  <si>
-    <t>push registers to stack</t>
-  </si>
-  <si>
-    <t>set dcsr[ebreakm]=1</t>
-  </si>
-  <si>
-    <t>fix mepc to skip over the wfi</t>
-  </si>
-  <si>
-    <t>pop registers from stack</t>
-  </si>
-  <si>
-    <t>dret</t>
-  </si>
-  <si>
-    <t>Second Debug handler:</t>
-  </si>
-  <si>
-    <t>Self checking code of mepc/mcause/etc.</t>
-  </si>
-  <si>
-    <t>Execution Steps:</t>
-  </si>
-  <si>
-    <t>1) main code executes and sleeps on wfi</t>
-  </si>
-  <si>
-    <t>2) trigger first handler by setting riscv_core input  debug_req_i=1</t>
-  </si>
-  <si>
-    <t>3) First debug handler completes</t>
-  </si>
-  <si>
-    <t>4) Set riscv_core input debug_req_i=0 before main code executes EBREAK</t>
-  </si>
-  <si>
-    <t>5) main code resumes and eventually executes EBREAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6) Execution of second debug handler occurs due to EBREAK </t>
-  </si>
-  <si>
     <t>No exceptions occur on access of mtval, writes are ignored, and reads return 0</t>
   </si>
   <si>
@@ -701,12 +625,6 @@
 exceptions</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>DPC</t>
   </si>
   <si>
@@ -741,315 +659,6 @@
   </si>
   <si>
     <t>Debug mode is entered at correct PC value and instruction at that value is executed upon dret</t>
-  </si>
-  <si>
-    <t>CSR name</t>
-  </si>
-  <si>
-    <t>CSR address</t>
-  </si>
-  <si>
-    <t>WARL bitfields?</t>
-  </si>
-  <si>
-    <t>WARA bitfields?</t>
-  </si>
-  <si>
-    <t>mstatus</t>
-  </si>
-  <si>
-    <t>0x300</t>
-  </si>
-  <si>
-    <t>0x301</t>
-  </si>
-  <si>
-    <t>misa</t>
-  </si>
-  <si>
-    <t>0x304</t>
-  </si>
-  <si>
-    <t>mie</t>
-  </si>
-  <si>
-    <t>0x305</t>
-  </si>
-  <si>
-    <t>mtvec</t>
-  </si>
-  <si>
-    <t>0x306</t>
-  </si>
-  <si>
-    <t>mcounteren</t>
-  </si>
-  <si>
-    <t>0x340</t>
-  </si>
-  <si>
-    <t>mscratch</t>
-  </si>
-  <si>
-    <t>0x341</t>
-  </si>
-  <si>
-    <t>mepc</t>
-  </si>
-  <si>
-    <t>0x342</t>
-  </si>
-  <si>
-    <t>mcause</t>
-  </si>
-  <si>
-    <t>0x343</t>
-  </si>
-  <si>
-    <t>mtval</t>
-  </si>
-  <si>
-    <t>0x344</t>
-  </si>
-  <si>
-    <t>mip</t>
-  </si>
-  <si>
-    <t>0x346</t>
-  </si>
-  <si>
-    <t>mintstatus</t>
-  </si>
-  <si>
-    <t>0x7A0</t>
-  </si>
-  <si>
-    <t>tselect</t>
-  </si>
-  <si>
-    <t>0x7A1</t>
-  </si>
-  <si>
-    <t>tdata1</t>
-  </si>
-  <si>
-    <t>0x7A2</t>
-  </si>
-  <si>
-    <t>tdata2</t>
-  </si>
-  <si>
-    <t>0x7A3</t>
-  </si>
-  <si>
-    <t>tdata3</t>
-  </si>
-  <si>
-    <t>0x7A4</t>
-  </si>
-  <si>
-    <t>tinfo</t>
-  </si>
-  <si>
-    <t>0x7A8</t>
-  </si>
-  <si>
-    <t>mcontext</t>
-  </si>
-  <si>
-    <t>0x7AA</t>
-  </si>
-  <si>
-    <t>scontext</t>
-  </si>
-  <si>
-    <t>0x7B0</t>
-  </si>
-  <si>
-    <t>dcsr</t>
-  </si>
-  <si>
-    <t>0x7B1</t>
-  </si>
-  <si>
-    <t>dpc</t>
-  </si>
-  <si>
-    <t>0x7B2</t>
-  </si>
-  <si>
-    <t>dscratch0</t>
-  </si>
-  <si>
-    <t>0x7B3</t>
-  </si>
-  <si>
-    <t>dscratch1</t>
-  </si>
-  <si>
-    <t>0x7C0</t>
-  </si>
-  <si>
-    <t>lpstart0</t>
-  </si>
-  <si>
-    <t>0x7C1</t>
-  </si>
-  <si>
-    <t>lpend0</t>
-  </si>
-  <si>
-    <t>0x7C2</t>
-  </si>
-  <si>
-    <t>lpcount0</t>
-  </si>
-  <si>
-    <t>0x7C4</t>
-  </si>
-  <si>
-    <t>lpstart1</t>
-  </si>
-  <si>
-    <t>0x7C5</t>
-  </si>
-  <si>
-    <t>lpend1</t>
-  </si>
-  <si>
-    <t>0x7C6</t>
-  </si>
-  <si>
-    <t>lpcount1</t>
-  </si>
-  <si>
-    <t>0xF11</t>
-  </si>
-  <si>
-    <t>0xF12</t>
-  </si>
-  <si>
-    <t>0xF13</t>
-  </si>
-  <si>
-    <t>0xF14</t>
-  </si>
-  <si>
-    <t>mvendorid</t>
-  </si>
-  <si>
-    <t>marchid</t>
-  </si>
-  <si>
-    <t>mimpid</t>
-  </si>
-  <si>
-    <t>mhartid</t>
-  </si>
-  <si>
-    <t>[31:0]</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>All bitfields 1 bit wide, covered by writing 0xFFFFFFFF and 0x00000000</t>
-  </si>
-  <si>
-    <t>Writes ignored, reads return 0</t>
-  </si>
-  <si>
-    <t>Read only, hardwired to 0</t>
-  </si>
-  <si>
-    <t>[31:2]</t>
-  </si>
-  <si>
-    <t>alligned to 4096 bytes, [13:2] hardwired to 0, [31:14] WARA, [1:0] hardwired to 1</t>
-  </si>
-  <si>
-    <t>Scratch value, all writes are legal</t>
-  </si>
-  <si>
-    <t>Additional Testing?</t>
-  </si>
-  <si>
-    <t>Writes ignored, reads return PC of instruction exception/interrupt occurred during</t>
-  </si>
-  <si>
-    <t>Entire register is WLRL</t>
-  </si>
-  <si>
-    <t>Read only</t>
-  </si>
-  <si>
-    <t>All writes legal</t>
-  </si>
-  <si>
-    <t>always reads as 0 since there's only 1 trigger</t>
-  </si>
-  <si>
-    <t>[2]</t>
-  </si>
-  <si>
-    <t>[7], [4], [3], [0]</t>
-  </si>
-  <si>
-    <t>Single bitfield, all values tested during debug trigger testing, bitfield can only be written in debug mode</t>
-  </si>
-  <si>
-    <t>Can only be written in debug mode</t>
-  </si>
-  <si>
-    <t>[15], [12], [11], [2]</t>
-  </si>
-  <si>
-    <t>All writeable bitfields 1 bit wide, covered by writing 0xFFFFFFFF and 0x00000000</t>
-  </si>
-  <si>
-    <t>Writes are legal and set next instruction after debug mode</t>
-  </si>
-  <si>
-    <t>RLWI bitfields?</t>
-  </si>
-  <si>
-    <t>Note:</t>
-  </si>
-  <si>
-    <t>WARL =</t>
-  </si>
-  <si>
-    <t>Write any, read legal</t>
-  </si>
-  <si>
-    <t>WARA =</t>
-  </si>
-  <si>
-    <t>write any, read any</t>
-  </si>
-  <si>
-    <t>RLWI =</t>
-  </si>
-  <si>
-    <t>Read legal, write ignored</t>
-  </si>
-  <si>
-    <t>All others</t>
-  </si>
-  <si>
-    <t>[1:0]</t>
-  </si>
-  <si>
-    <t>[31:16], [7:0]</t>
-  </si>
-  <si>
-    <t>[31:3], [1:0]</t>
-  </si>
-  <si>
-    <t>[31:28], [1:0]</t>
   </si>
   <si>
     <t>When debug mode is entered, contains the address of the next instruction to be executed</t>
@@ -1105,6 +714,15 @@
   </si>
   <si>
     <t>https://core-v-docs-verif-strat.readthedocs.io/projects/cv32e40p_um/en/latest/</t>
+  </si>
+  <si>
+    <t>Functional Coverage</t>
+  </si>
+  <si>
+    <t>Show that mcause is the correct value upon reset (0x00000000)</t>
+  </si>
+  <si>
+    <t>Reset sets mcause to 0x00000000</t>
   </si>
 </sst>
 </file>
@@ -1157,18 +775,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1215,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1246,23 +865,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1554,8 +1182,14 @@
   <threadedComment ref="B2" dT="2020-09-11T17:55:59.20" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{37ABB1D9-DB03-45ED-AFAD-55734EBCB3C8}">
     <text>Its not clear that this a feature of CV32E40P.  I've open issue #497 to find out.</text>
   </threadedComment>
+  <threadedComment ref="B2" dT="2020-09-15T22:16:56.87" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{233B4665-9EA8-41F6-9027-E905DE3A5B23}" parentId="{37ABB1D9-DB03-45ED-AFAD-55734EBCB3C8}">
+    <text>Need to add the concept of "non-existant addresses" in the testbench memory.</text>
+  </threadedComment>
   <threadedComment ref="B3" dT="2020-09-11T17:58:19.14" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{FD0C4767-67A6-4F9E-8956-3FCB07F9ED56}">
     <text>How do we present illegal instructions to the core?  Will the Google ISG actually generate illegal instructions?   How are these handled by the toolchain?</text>
+  </threadedComment>
+  <threadedComment ref="B3" dT="2020-09-15T22:28:36.32" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{2BA0BFDD-53F3-43B0-AEA3-466324435A06}" parentId="{FD0C4767-67A6-4F9E-8956-3FCB07F9ED56}">
+    <text>David has a script that deliberately generates mis-formed instructions.</text>
   </threadedComment>
   <threadedComment ref="B4" dT="2020-09-11T17:59:14.23" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{9D2A13B5-1671-4066-99D0-5AAEE72AF6AF}">
     <text>If we had full coverage of the supported instructions of the ISA, would this not suffice?</text>
@@ -1563,8 +1197,14 @@
   <threadedComment ref="D5" dT="2020-09-11T19:54:51.19" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{9322B244-D970-433D-A518-EDE71E407481}">
     <text>Question: can your test-program throw an error if an unexpected exception occurs?   Throw an error if an expected exception does not occur?</text>
   </threadedComment>
+  <threadedComment ref="D5" dT="2020-09-15T22:32:57.72" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{5ECAC549-60BC-4F99-B904-509D82C80A9B}" parentId="{9322B244-D970-433D-A518-EDE71E407481}">
+    <text>Not required - ISS will mis-match on mepc</text>
+  </threadedComment>
   <threadedComment ref="G6" dT="2020-09-11T19:56:03.63" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{2406D81D-9721-4D0D-B869-47006E696B60}">
     <text>Idealy we would have functional coverage on the Instruction fetch bus to cover these specific scenarios.</text>
+  </threadedComment>
+  <threadedComment ref="G6" dT="2020-09-15T22:36:06.39" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{CB99B7E0-6559-43DD-AB9E-6AFD01B41F8F}" parentId="{2406D81D-9721-4D0D-B869-47006E696B60}">
+    <text>All agreed.</text>
   </threadedComment>
   <threadedComment ref="B8" dT="2020-09-11T19:56:49.27" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{4AD939A8-000B-4C00-9781-6690334399AA}">
     <text>I would recommend we track this in the CSR DV plan.  Same for Features in rows 9..11.</text>
@@ -1584,19 +1224,16 @@
   <threadedComment ref="B21" dT="2020-09-11T20:04:27.00" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{89B78706-C4A4-4214-92F5-A0D38D74FF9E}">
     <text>I like this Feature, but its not clear how the test-program is implemented.</text>
   </threadedComment>
-  <threadedComment ref="C23" dT="2020-09-11T20:08:06.28" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{F5DE54AA-7939-4D93-9554-653FB95AB5D1}">
+  <threadedComment ref="B21" dT="2020-09-15T22:45:27.14" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{8B96A442-B57E-40F8-9FB9-4E8167467445}" parentId="{89B78706-C4A4-4214-92F5-A0D38D74FF9E}">
+    <text>Two options: (1) encode the expected exception in the handler, or (2) compare against RM.</text>
+  </threadedComment>
+  <threadedComment ref="C23" dT="2020-09-11T20:08:06.28" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{F5DE54AA-7939-4D93-9554-653FB95AB5D1}" done="1">
     <text>Ordinarily this would be part of a CSR DV plan, but getting bits set in mcause is better done as part of the exceptions DV plan.</text>
   </threadedComment>
-  <threadedComment ref="D23" dT="2020-09-11T20:09:03.49" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{B5686705-6936-4530-B6D0-3F3CD5963FE2}">
-    <text>PoR value of mstatus is 0x1800.  PoR of mcause is 0x0.</text>
-  </threadedComment>
-  <threadedComment ref="E23" dT="2020-09-11T20:09:49.50" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{6E6FDA3F-C3C0-43D6-ADD6-7422FC32A68B}">
-    <text>This should be reset after some exception causes mcause to be non-zero.</text>
-  </threadedComment>
-  <threadedComment ref="B24" dT="2020-09-11T20:11:14.34" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{4D7114F4-5E6B-4775-AE24-3DDEAA3CDBB2}">
+  <threadedComment ref="B24" dT="2020-09-11T20:11:14.34" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{4D7114F4-5E6B-4775-AE24-3DDEAA3CDBB2}" done="1">
     <text>Debug DV plan</text>
   </threadedComment>
-  <threadedComment ref="B25" dT="2020-09-11T20:10:58.56" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{E64922F1-6739-4F8C-9676-630AF88E031E}">
+  <threadedComment ref="B25" dT="2020-09-11T20:10:58.56" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{E64922F1-6739-4F8C-9676-630AF88E031E}" done="1">
     <text>Debug DV plan</text>
   </threadedComment>
   <threadedComment ref="B26" dT="2020-09-11T20:10:27.49" personId="{18966CCC-7A4D-428E-A9A3-E332B66BAE32}" id="{09651DE0-A277-480B-A8D0-FD376075F849}">
@@ -1614,7 +1251,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1263,7 @@
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" style="12" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="78.140625" customWidth="1"/>
   </cols>
@@ -1653,8 +1290,8 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>284</v>
+      <c r="H1" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1667,13 +1304,13 @@
         <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -1681,7 +1318,7 @@
       <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="12"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1692,13 +1329,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>285</v>
+        <v>158</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
         <v>43</v>
@@ -1706,31 +1343,31 @@
       <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D4" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1741,13 +1378,13 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -1755,7 +1392,7 @@
       <c r="G5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1765,19 +1402,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -1791,13 +1428,13 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -1805,30 +1442,30 @@
       <c r="G7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H8" s="11"/>
@@ -1839,22 +1476,22 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>44</v>
       </c>
       <c r="H9" s="11"/>
@@ -1865,22 +1502,22 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="D10" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="17" t="s">
         <v>44</v>
       </c>
       <c r="H10" s="11"/>
@@ -1891,22 +1528,22 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="C11" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H11" s="11"/>
@@ -1917,22 +1554,22 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H12" s="11"/>
@@ -1940,19 +1577,19 @@
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>283</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>7</v>
@@ -1966,19 +1603,19 @@
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>290</v>
+        <v>163</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>7</v>
@@ -1998,13 +1635,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>7</v>
@@ -2024,13 +1661,13 @@
         <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>7</v>
@@ -2044,24 +1681,24 @@
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="C17" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H17" s="11"/>
@@ -2076,13 +1713,13 @@
         <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>7</v>
@@ -2102,13 +1739,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>7</v>
@@ -2124,22 +1761,22 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H20" s="11"/>
@@ -2148,19 +1785,19 @@
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>7</v>
@@ -2174,19 +1811,19 @@
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>7</v>
@@ -2209,10 +1846,10 @@
         <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>7</v>
@@ -2225,24 +1862,24 @@
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="17" t="s">
         <v>44</v>
       </c>
       <c r="H24" s="11"/>
@@ -2251,24 +1888,24 @@
     </row>
     <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="17" t="s">
         <v>44</v>
       </c>
       <c r="H25" s="11"/>
@@ -2277,19 +1914,19 @@
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>280</v>
+        <v>153</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>281</v>
+        <v>154</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>282</v>
+        <v>155</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>7</v>
@@ -2302,19 +1939,19 @@
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>277</v>
+        <v>150</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>278</v>
+        <v>151</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>279</v>
+        <v>152</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>7</v>
@@ -2336,45 +1973,45 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" s="13"/>
+        <v>129</v>
+      </c>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" s="13"/>
+        <v>130</v>
+      </c>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="13"/>
+        <v>131</v>
+      </c>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>294</v>
-      </c>
-      <c r="F33" s="13"/>
+        <v>167</v>
+      </c>
+      <c r="F33" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2388,7 +2025,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,48 +2039,48 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20" t="s">
+      <c r="A5" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -2455,14 +2092,14 @@
       <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="20">
         <v>0</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,14 +2112,14 @@
       <c r="C8" s="8">
         <v>0</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="21">
         <v>0</v>
       </c>
       <c r="E8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2495,14 +2132,14 @@
       <c r="C9" s="8">
         <v>0</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="21">
         <v>1</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2515,14 +2152,14 @@
       <c r="C10" s="5">
         <v>0</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="20">
         <v>1</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2535,14 +2172,14 @@
       <c r="C11" s="8">
         <v>1</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="21">
         <v>0</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2555,14 +2192,14 @@
       <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="22">
         <v>0</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2575,14 +2212,14 @@
       <c r="C13" s="7">
         <v>1</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="22">
         <v>1</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2595,14 +2232,14 @@
       <c r="C14" s="5">
         <v>1</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="20">
         <v>1</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2615,14 +2252,14 @@
       <c r="C15" s="8">
         <v>0</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="21">
         <v>0</v>
       </c>
       <c r="E15" s="8">
         <v>0</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2635,14 +2272,14 @@
       <c r="C16" s="5">
         <v>0</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="20">
         <v>0</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2655,14 +2292,14 @@
       <c r="C17" s="5">
         <v>0</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="20">
         <v>1</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,34 +2312,34 @@
       <c r="C18" s="5">
         <v>0</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="20">
         <v>1</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <v>0</v>
-      </c>
-      <c r="B19" s="15">
-        <v>1</v>
-      </c>
-      <c r="C19" s="15">
-        <v>1</v>
-      </c>
-      <c r="D19" s="15">
-        <v>0</v>
-      </c>
-      <c r="E19" s="15">
+      <c r="A19" s="14">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14">
+        <v>1</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="23">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14">
         <v>0</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2715,14 +2352,14 @@
       <c r="C20" s="5">
         <v>1</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="20">
         <v>0</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2735,14 +2372,14 @@
       <c r="C21" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="20">
         <v>1</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,14 +2392,14 @@
       <c r="C22" s="5">
         <v>1</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="20">
         <v>1</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,14 +2412,14 @@
       <c r="C23" s="8">
         <v>0</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="21">
         <v>0</v>
       </c>
       <c r="E23" s="8">
         <v>0</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,14 +2432,14 @@
       <c r="C24" s="5">
         <v>0</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="20">
         <v>0</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2815,14 +2452,14 @@
       <c r="C25" s="5">
         <v>0</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="20">
         <v>1</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2835,14 +2472,14 @@
       <c r="C26" s="5">
         <v>0</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="20">
         <v>1</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2855,14 +2492,14 @@
       <c r="C27" s="7">
         <v>1</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="22">
         <v>0</v>
       </c>
       <c r="E27" s="7">
         <v>0</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2875,14 +2512,14 @@
       <c r="C28" s="5">
         <v>1</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="20">
         <v>0</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2895,14 +2532,14 @@
       <c r="C29" s="5">
         <v>1</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="20">
         <v>1</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2915,14 +2552,14 @@
       <c r="C30" s="5">
         <v>1</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="20">
         <v>1</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2935,14 +2572,14 @@
       <c r="C31" s="5">
         <v>0</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="20">
         <v>0</v>
       </c>
       <c r="E31" s="5">
         <v>0</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,14 +2592,14 @@
       <c r="C32" s="5">
         <v>0</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="20">
         <v>0</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2975,14 +2612,14 @@
       <c r="C33" s="5">
         <v>0</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="20">
         <v>1</v>
       </c>
       <c r="E33" s="5">
         <v>0</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2995,14 +2632,14 @@
       <c r="C34" s="5">
         <v>0</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="20">
         <v>1</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3015,14 +2652,14 @@
       <c r="C35" s="5">
         <v>1</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="20">
         <v>0</v>
       </c>
       <c r="E35" s="5">
         <v>0</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3035,14 +2672,14 @@
       <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="20">
         <v>0</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3055,14 +2692,14 @@
       <c r="C37" s="5">
         <v>1</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="20">
         <v>1</v>
       </c>
       <c r="E37" s="5">
         <v>0</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -3075,14 +2712,14 @@
       <c r="C38" s="5">
         <v>1</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="20">
         <v>1</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3092,965 +2729,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="95.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D4" t="s">
-        <v>243</v>
-      </c>
-      <c r="E4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" t="s">
-        <v>243</v>
-      </c>
-      <c r="D5" t="s">
-        <v>248</v>
-      </c>
-      <c r="E5" t="s">
-        <v>273</v>
-      </c>
-      <c r="F5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F6" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D7" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" t="s">
-        <v>243</v>
-      </c>
-      <c r="F7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D8" t="s">
-        <v>242</v>
-      </c>
-      <c r="E8" t="s">
-        <v>243</v>
-      </c>
-      <c r="F8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" t="s">
-        <v>243</v>
-      </c>
-      <c r="D9" t="s">
-        <v>243</v>
-      </c>
-      <c r="E9" t="s">
-        <v>242</v>
-      </c>
-      <c r="F9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" t="s">
-        <v>243</v>
-      </c>
-      <c r="D10" t="s">
-        <v>243</v>
-      </c>
-      <c r="E10" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" t="s">
-        <v>243</v>
-      </c>
-      <c r="D11" t="s">
-        <v>243</v>
-      </c>
-      <c r="E11" t="s">
-        <v>242</v>
-      </c>
-      <c r="F11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E12" t="s">
-        <v>274</v>
-      </c>
-      <c r="F12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B13" t="s">
-        <v>201</v>
-      </c>
-      <c r="C13" t="s">
-        <v>243</v>
-      </c>
-      <c r="D13" t="s">
-        <v>243</v>
-      </c>
-      <c r="E13" t="s">
-        <v>242</v>
-      </c>
-      <c r="F13" t="s">
-        <v>161</v>
-      </c>
-      <c r="G13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>202</v>
-      </c>
-      <c r="B14" t="s">
-        <v>203</v>
-      </c>
-      <c r="C14" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" t="s">
-        <v>257</v>
-      </c>
-      <c r="E14" t="s">
-        <v>275</v>
-      </c>
-      <c r="F14" t="s">
-        <v>161</v>
-      </c>
-      <c r="G14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>204</v>
-      </c>
-      <c r="B15" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E15" t="s">
-        <v>243</v>
-      </c>
-      <c r="F15" t="s">
-        <v>160</v>
-      </c>
-      <c r="G15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C16" t="s">
-        <v>243</v>
-      </c>
-      <c r="D16" t="s">
-        <v>243</v>
-      </c>
-      <c r="E16" t="s">
-        <v>242</v>
-      </c>
-      <c r="F16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>208</v>
-      </c>
-      <c r="B17" t="s">
-        <v>209</v>
-      </c>
-      <c r="C17" t="s">
-        <v>243</v>
-      </c>
-      <c r="D17" t="s">
-        <v>243</v>
-      </c>
-      <c r="E17" t="s">
-        <v>242</v>
-      </c>
-      <c r="F17" t="s">
-        <v>161</v>
-      </c>
-      <c r="G17" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>210</v>
-      </c>
-      <c r="B18" t="s">
-        <v>211</v>
-      </c>
-      <c r="C18" t="s">
-        <v>243</v>
-      </c>
-      <c r="D18" t="s">
-        <v>243</v>
-      </c>
-      <c r="E18" t="s">
-        <v>242</v>
-      </c>
-      <c r="F18" t="s">
-        <v>161</v>
-      </c>
-      <c r="G18" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>212</v>
-      </c>
-      <c r="B19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" t="s">
-        <v>243</v>
-      </c>
-      <c r="D19" t="s">
-        <v>243</v>
-      </c>
-      <c r="E19" t="s">
-        <v>242</v>
-      </c>
-      <c r="F19" t="s">
-        <v>161</v>
-      </c>
-      <c r="G19" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>214</v>
-      </c>
-      <c r="B20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" t="s">
-        <v>243</v>
-      </c>
-      <c r="D20" t="s">
-        <v>261</v>
-      </c>
-      <c r="E20" t="s">
-        <v>276</v>
-      </c>
-      <c r="F20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G20" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" t="s">
-        <v>243</v>
-      </c>
-      <c r="D21" t="s">
-        <v>242</v>
-      </c>
-      <c r="E21" t="s">
-        <v>243</v>
-      </c>
-      <c r="F21" t="s">
-        <v>161</v>
-      </c>
-      <c r="G21" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" t="s">
-        <v>219</v>
-      </c>
-      <c r="C22" t="s">
-        <v>243</v>
-      </c>
-      <c r="D22" t="s">
-        <v>242</v>
-      </c>
-      <c r="E22" t="s">
-        <v>243</v>
-      </c>
-      <c r="F22" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>220</v>
-      </c>
-      <c r="B23" t="s">
-        <v>221</v>
-      </c>
-      <c r="C23" t="s">
-        <v>243</v>
-      </c>
-      <c r="D23" t="s">
-        <v>242</v>
-      </c>
-      <c r="E23" t="s">
-        <v>243</v>
-      </c>
-      <c r="F23" t="s">
-        <v>161</v>
-      </c>
-      <c r="G23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>222</v>
-      </c>
-      <c r="B24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D24" t="s">
-        <v>242</v>
-      </c>
-      <c r="E24" t="s">
-        <v>243</v>
-      </c>
-      <c r="F24" t="s">
-        <v>160</v>
-      </c>
-      <c r="G24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>224</v>
-      </c>
-      <c r="B25" t="s">
-        <v>225</v>
-      </c>
-      <c r="C25" t="s">
-        <v>243</v>
-      </c>
-      <c r="D25" t="s">
-        <v>242</v>
-      </c>
-      <c r="E25" t="s">
-        <v>243</v>
-      </c>
-      <c r="F25" t="s">
-        <v>160</v>
-      </c>
-      <c r="G25" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B26" t="s">
-        <v>227</v>
-      </c>
-      <c r="C26" t="s">
-        <v>243</v>
-      </c>
-      <c r="D26" t="s">
-        <v>242</v>
-      </c>
-      <c r="E26" t="s">
-        <v>243</v>
-      </c>
-      <c r="F26" t="s">
-        <v>160</v>
-      </c>
-      <c r="G26" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>228</v>
-      </c>
-      <c r="B27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C27" t="s">
-        <v>243</v>
-      </c>
-      <c r="D27" t="s">
-        <v>242</v>
-      </c>
-      <c r="E27" t="s">
-        <v>243</v>
-      </c>
-      <c r="F27" t="s">
-        <v>160</v>
-      </c>
-      <c r="G27" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>230</v>
-      </c>
-      <c r="B28" t="s">
-        <v>231</v>
-      </c>
-      <c r="C28" t="s">
-        <v>243</v>
-      </c>
-      <c r="D28" t="s">
-        <v>242</v>
-      </c>
-      <c r="E28" t="s">
-        <v>243</v>
-      </c>
-      <c r="F28" t="s">
-        <v>160</v>
-      </c>
-      <c r="G28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>232</v>
-      </c>
-      <c r="B29" t="s">
-        <v>233</v>
-      </c>
-      <c r="C29" t="s">
-        <v>243</v>
-      </c>
-      <c r="D29" t="s">
-        <v>242</v>
-      </c>
-      <c r="E29" t="s">
-        <v>243</v>
-      </c>
-      <c r="F29" t="s">
-        <v>160</v>
-      </c>
-      <c r="G29" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>234</v>
-      </c>
-      <c r="B30" t="s">
-        <v>238</v>
-      </c>
-      <c r="C30" t="s">
-        <v>243</v>
-      </c>
-      <c r="D30" t="s">
-        <v>243</v>
-      </c>
-      <c r="E30" t="s">
-        <v>242</v>
-      </c>
-      <c r="F30" t="s">
-        <v>161</v>
-      </c>
-      <c r="G30" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>235</v>
-      </c>
-      <c r="B31" t="s">
-        <v>239</v>
-      </c>
-      <c r="C31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D31" t="s">
-        <v>243</v>
-      </c>
-      <c r="E31" t="s">
-        <v>242</v>
-      </c>
-      <c r="F31" t="s">
-        <v>161</v>
-      </c>
-      <c r="G31" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" t="s">
-        <v>240</v>
-      </c>
-      <c r="C32" t="s">
-        <v>243</v>
-      </c>
-      <c r="D32" t="s">
-        <v>243</v>
-      </c>
-      <c r="E32" t="s">
-        <v>242</v>
-      </c>
-      <c r="F32" t="s">
-        <v>161</v>
-      </c>
-      <c r="G32" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>237</v>
-      </c>
-      <c r="B33" t="s">
-        <v>241</v>
-      </c>
-      <c r="C33" t="s">
-        <v>243</v>
-      </c>
-      <c r="D33" t="s">
-        <v>243</v>
-      </c>
-      <c r="E33" t="s">
-        <v>242</v>
-      </c>
-      <c r="F33" t="s">
-        <v>161</v>
-      </c>
-      <c r="G33" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>266</v>
-      </c>
-      <c r="B36" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>268</v>
-      </c>
-      <c r="B37" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>270</v>
-      </c>
-      <c r="B38" t="s">
-        <v>271</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>